<commit_message>
feat: update template file
</commit_message>
<xml_diff>
--- a/public/template/CPE_course_import_template.xlsx
+++ b/public/template/CPE_course_import_template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Desktop\CPE 402\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inu-garden\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9909BB-A99E-4BC2-B332-53657C026C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C824CB-B2F3-426B-A60A-C6FBFBD1EC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14910" xr2:uid="{898897A6-CF24-E645-BCDA-42942615C977}"/>
   </bookViews>
   <sheets>
     <sheet name="(IN) PO and CLO" sheetId="2" r:id="rId1"/>
-    <sheet name="(IN) StudentList" sheetId="16" r:id="rId2"/>
-    <sheet name="(IN) WeeklyPlan" sheetId="19" r:id="rId3"/>
+    <sheet name="(IN) WeeklyPlan" sheetId="19" r:id="rId2"/>
+    <sheet name="(IN) StudentList" sheetId="16" r:id="rId3"/>
     <sheet name="(IN) RawScores" sheetId="20" r:id="rId4"/>
     <sheet name="Course Catalogue" sheetId="12" r:id="rId5"/>
     <sheet name="Reference-TABEE_POs" sheetId="25" r:id="rId6"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="201">
   <si>
     <t>Topics</t>
   </si>
@@ -696,6 +696,9 @@
   </si>
   <si>
     <t>* ข้อมูลต้องมีครบ 4 ตัว</t>
+  </si>
+  <si>
+    <t>* ใส่ปีเป็น พ.ศ.</t>
   </si>
 </sst>
 </file>
@@ -2761,22 +2764,6 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D7A935DE-D62D-1743-A5BF-26ACBA295F37}" name="StudentList" displayName="StudentList" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{D7A935DE-D62D-1743-A5BF-26ACBA295F37}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{27B0D223-3521-AB44-8B0A-0368A4082BED}" name="Seq No."/>
-    <tableColumn id="2" xr3:uid="{8F06A4C6-A54F-3641-AAB7-7359C8717A6E}" name="Student Code"/>
-    <tableColumn id="3" xr3:uid="{31F76B75-6931-E742-8C27-2160A39B3BFF}" name="Student Name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDF583EC-A057-3E4E-AC1C-7F24FDF5E16B}" name="WeeklyPlan" displayName="WeeklyPlan" ref="A1:L6" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A1:L6" xr:uid="{EDF583EC-A057-3E4E-AC1C-7F24FDF5E16B}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2807,6 +2794,22 @@
     <tableColumn id="13" xr3:uid="{621295FD-94A6-1A40-AE90-78446C01FBDD}" name="Learning Activity" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D7A935DE-D62D-1743-A5BF-26ACBA295F37}" name="StudentList" displayName="StudentList" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3" xr:uid="{D7A935DE-D62D-1743-A5BF-26ACBA295F37}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{27B0D223-3521-AB44-8B0A-0368A4082BED}" name="Seq No."/>
+    <tableColumn id="2" xr3:uid="{8F06A4C6-A54F-3641-AAB7-7359C8717A6E}" name="Student Code"/>
+    <tableColumn id="3" xr3:uid="{31F76B75-6931-E742-8C27-2160A39B3BFF}" name="Student Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3146,7 +3149,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -3247,6 +3250,9 @@
       <c r="E6" s="24">
         <v>2.2000000000000002</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="9"/>
@@ -3417,7 +3423,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="8">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C6" xr:uid="{AE689283-4B7C-D64A-9C50-909FAF115A9A}">
       <formula1>"Knowledge, Skills, Attitude"</formula1>
     </dataValidation>
@@ -3433,7 +3439,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6" xr:uid="{F3958E12-9BDE-3740-A06A-428FB9E34742}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G2" xr:uid="{BE2F403F-AF11-F448-90C3-EDE8310AE4FF}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{BE2F403F-AF11-F448-90C3-EDE8310AE4FF}">
       <formula1>2019</formula1>
       <formula2>2050</formula2>
     </dataValidation>
@@ -3443,6 +3449,14 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C14 C18:C21" xr:uid="{81D50489-C238-884C-A643-B6BE0B2E1AE5}">
       <formula1>0</formula1>
       <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{44909829-D005-475A-AF7F-7E8D0D78F32C}">
+      <formula1>2500</formula1>
+      <formula2>2700</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{E1919CD2-8DDB-40E7-80CB-B69BBEA7DCCC}">
+      <formula1>2500</formula1>
+      <formula2>2600</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3457,78 +3471,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DB371C-8BD0-C242-B6C8-5194D8541877}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>62070500000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>62070500001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="E5" s="38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731C9897-4851-3C4B-A0EF-A9BF30D27A38}">
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15"/>
@@ -4105,6 +4053,72 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DB371C-8BD0-C242-B6C8-5194D8541877}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>62070500000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>62070500001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="E5" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>